<commit_message>
pre activation edit,delete,duplicate complete
</commit_message>
<xml_diff>
--- a/uploads/import_chat_ids.xlsx
+++ b/uploads/import_chat_ids.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usman\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usman\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,19 +33,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF545454"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,9 +62,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,16 +344,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -368,102 +358,56 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>5141281331</v>
+      <c r="A2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>5141281332</v>
+      <c r="A3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>5141281333</v>
+      <c r="A4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>5141281334</v>
+      <c r="A5">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5141281335</v>
+      <c r="A6">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5141281336</v>
+      <c r="A7">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>5141281337</v>
+      <c r="A8">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>5141281338</v>
+      <c r="A9">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>5141281339</v>
+      <c r="A10">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>5141281340</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>5141281341</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>5141281342</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>5141281343</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>5141281344</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>5141281345</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>5141281346</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>5141281347</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>5141281348</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>5141281349</v>
+      <c r="A11">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>